<commit_message>
Alberta Transformers and Workspaces / Major Update
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/AB_DefaultAttributeMapper.xlsx
+++ b/FME_files/LOOKUP_TABLES/AB_DefaultAttributeMapper.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\LOOKUP_TABLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robennet\Documents\GitHub\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="5610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="3360"/>
   </bookViews>
   <sheets>
     <sheet name="AB_DEFAULT_ATTRIBUTES" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t>p-t_entity</t>
   </si>
@@ -80,56 +80,166 @@
     <t>default_progress_value</t>
   </si>
   <si>
+    <t>default_topic_value</t>
+  </si>
+  <si>
+    <t>default_tag_value</t>
+  </si>
+  <si>
+    <t>Alberta Data</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>vector</t>
+  </si>
+  <si>
+    <t>geoscientificInformation</t>
+  </si>
+  <si>
+    <t>onGoing</t>
+  </si>
+  <si>
+    <t>abstract_other_lang_value</t>
+  </si>
+  <si>
+    <t>#fra</t>
+  </si>
+  <si>
+    <t>contact_position_other_lang_locale</t>
+  </si>
+  <si>
+    <t>p-t_entity_other_lang_locale</t>
+  </si>
+  <si>
+    <t>contact_email_other_lang_locale</t>
+  </si>
+  <si>
+    <t>keyword_other_lang_locale</t>
+  </si>
+  <si>
+    <t>reference_system</t>
+  </si>
+  <si>
+    <t>reference_system_version</t>
+  </si>
+  <si>
+    <t>dataset_title_other_lang_locale</t>
+  </si>
+  <si>
+    <t>abstract_other_lang_warning</t>
+  </si>
+  <si>
+    <t>** Cet élément de métadonnées provenant d’une tierce partie a été traduit à l'aide d'un outil de traduction automatisée (Amazon Translate). Pour signaler toute anomalie, veuillez communiquer avec nous à nrcan.fgp-pgf.rncan@canada.ca **</t>
+  </si>
+  <si>
+    <t>abstract_other_lang_locale</t>
+  </si>
+  <si>
+    <t>service_other_lang_locale</t>
+  </si>
+  <si>
+    <t>p-t_license_other_lang_locale</t>
+  </si>
+  <si>
+    <t>default_update_value</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>default_distribution_format_version</t>
+  </si>
+  <si>
+    <t>14th fl Oxbridge Place,9820 - 106 Street NW</t>
+  </si>
+  <si>
+    <t>Edmonton</t>
+  </si>
+  <si>
+    <t>Alberta</t>
+  </si>
+  <si>
+    <t>geodiscoveralberta@gov.ab.ca</t>
+  </si>
+  <si>
+    <t>default_contact_address</t>
+  </si>
+  <si>
+    <t>default_contact_city</t>
+  </si>
+  <si>
+    <t>default_contact_email</t>
+  </si>
+  <si>
+    <t>default_contact_name</t>
+  </si>
+  <si>
+    <t>GeoDiscover Alberta</t>
+  </si>
+  <si>
+    <t>default_contact_position</t>
+  </si>
+  <si>
+    <t>The Provincial Geospatial Centre</t>
+  </si>
+  <si>
+    <t>default_contact_country</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>default_contact_administrative_area</t>
+  </si>
+  <si>
+    <t>default_contact_phone</t>
+  </si>
+  <si>
+    <t>T5K 2J6</t>
+  </si>
+  <si>
+    <t>1-780 -638-3172</t>
+  </si>
+  <si>
+    <t>default_contact_postal_code</t>
+  </si>
+  <si>
+    <t>transfer_option_name_other_lang_locale</t>
+  </si>
+  <si>
     <t>default_reference_code_value</t>
   </si>
   <si>
+    <t>EPSG: 3400</t>
+  </si>
+  <si>
     <t>default_reference_space_value</t>
   </si>
   <si>
-    <t>default_topic_value</t>
-  </si>
-  <si>
-    <t>default_tag_value</t>
-  </si>
-  <si>
-    <t>Alberta Data</t>
-  </si>
-  <si>
-    <t>EPSG: 3400</t>
-  </si>
-  <si>
     <t>EPSG</t>
   </si>
   <si>
     <t>default_reference_version_value</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>vector</t>
-  </si>
-  <si>
-    <t>geoscientificInformation</t>
-  </si>
-  <si>
-    <t>onGoing</t>
-  </si>
-  <si>
-    <t>default_update_value</t>
-  </si>
-  <si>
-    <t>asNeeded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,13 +262,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,13 +550,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
@@ -518,7 +631,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -526,7 +639,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -542,7 +655,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -555,29 +668,216 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B31" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>